<commit_message>
cleanup supplementary files and Western blot biological replicates plot
</commit_message>
<xml_diff>
--- a/Revisions/Supplementary_Files/Supplementary_FIle_5_gene_sets.xlsx
+++ b/Revisions/Supplementary_Files/Supplementary_FIle_5_gene_sets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tperica/Box Sync/kortemmelab/home/tina/Gsp1_manuscript/Revisions/Supplementary_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148F98BB-737C-C441-8D06-4C645A9F6234}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD4038B-4B9E-3540-ACDD-93965B7F4547}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1995,10 +1995,10 @@
     </r>
   </si>
   <si>
-    <t>Cluster from Fig. 4b  (1-7, or expanded dataset, see Methods)</t>
-  </si>
-  <si>
     <t>expanded dataset</t>
+  </si>
+  <si>
+    <t>actin, tubulin, and polarity</t>
   </si>
   <si>
     <r>
@@ -2033,11 +2033,11 @@
         <color theme="1"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve"> genes that have significant positive interactions with at least one of the Gsp1 mutants. Gene sets were made manually, based on biological functions of genes described in the SGD database.</t>
+      <t xml:space="preserve"> genes that have significant positive Pearson correlations of GI profiles with at least one of the Gsp1 mutants. Gene sets were made manually, based on biological functions of genes described in the SGD database.</t>
     </r>
   </si>
   <si>
-    <t>actin, tubulin, and polarity</t>
+    <t>Cluster from Fig. 4a  (1-7, or expanded dataset, see Methods)</t>
   </si>
 </sst>
 </file>
@@ -2496,7 +2496,7 @@
   <dimension ref="A1:D491"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2526,7 +2526,7 @@
         <v>648</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2848,7 +2848,7 @@
         <v>26</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -3100,7 +3100,7 @@
         <v>72</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -3324,7 +3324,7 @@
         <v>75</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -3366,7 +3366,7 @@
         <v>75</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -3380,7 +3380,7 @@
         <v>75</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -3548,7 +3548,7 @@
         <v>75</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -3576,7 +3576,7 @@
         <v>75</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -3912,7 +3912,7 @@
         <v>75</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -3926,7 +3926,7 @@
         <v>75</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -3996,7 +3996,7 @@
         <v>75</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -4066,7 +4066,7 @@
         <v>168</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -4262,7 +4262,7 @@
         <v>171</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -4276,7 +4276,7 @@
         <v>171</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -4304,7 +4304,7 @@
         <v>171</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -4332,7 +4332,7 @@
         <v>171</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -4346,7 +4346,7 @@
         <v>183</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -4360,7 +4360,7 @@
         <v>183</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -4402,7 +4402,7 @@
         <v>183</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
@@ -4430,7 +4430,7 @@
         <v>183</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -4626,7 +4626,7 @@
         <v>216</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -4679,7 +4679,7 @@
         <v>228</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D156" s="3">
         <v>7</v>
@@ -4693,10 +4693,10 @@
         <v>228</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -4707,7 +4707,7 @@
         <v>228</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D158" s="3">
         <v>7</v>
@@ -4721,10 +4721,10 @@
         <v>228</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -4735,10 +4735,10 @@
         <v>228</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -4749,7 +4749,7 @@
         <v>228</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D161" s="3">
         <v>7</v>
@@ -4763,7 +4763,7 @@
         <v>228</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D162" s="3">
         <v>7</v>
@@ -4777,7 +4777,7 @@
         <v>228</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D163" s="3">
         <v>7</v>
@@ -4791,10 +4791,10 @@
         <v>237</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -4805,7 +4805,7 @@
         <v>239</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D165" s="3">
         <v>7</v>
@@ -4819,7 +4819,7 @@
         <v>241</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D166" s="3">
         <v>7</v>
@@ -4833,7 +4833,7 @@
         <v>243</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D167" s="3">
         <v>7</v>
@@ -4847,7 +4847,7 @@
         <v>245</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D168" s="3">
         <v>7</v>
@@ -4861,10 +4861,10 @@
         <v>247</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
@@ -4875,7 +4875,7 @@
         <v>249</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D170" s="3">
         <v>4</v>
@@ -4889,7 +4889,7 @@
         <v>251</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D171" s="3">
         <v>7</v>
@@ -4903,7 +4903,7 @@
         <v>251</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D172" s="3">
         <v>7</v>
@@ -4917,10 +4917,10 @@
         <v>251</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
@@ -4931,7 +4931,7 @@
         <v>255</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D174" s="3">
         <v>4</v>
@@ -4945,7 +4945,7 @@
         <v>257</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D175" s="3">
         <v>7</v>
@@ -4959,7 +4959,7 @@
         <v>259</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D176" s="3">
         <v>7</v>
@@ -4973,7 +4973,7 @@
         <v>261</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D177" s="3">
         <v>6</v>
@@ -4987,10 +4987,10 @@
         <v>263</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
@@ -5001,7 +5001,7 @@
         <v>265</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D179" s="3">
         <v>7</v>
@@ -5032,7 +5032,7 @@
         <v>268</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
@@ -5046,7 +5046,7 @@
         <v>268</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
@@ -5060,7 +5060,7 @@
         <v>268</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
@@ -5116,7 +5116,7 @@
         <v>268</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
@@ -5130,7 +5130,7 @@
         <v>268</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
@@ -5144,7 +5144,7 @@
         <v>268</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
@@ -5200,7 +5200,7 @@
         <v>268</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
@@ -5228,7 +5228,7 @@
         <v>268</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
@@ -5242,7 +5242,7 @@
         <v>268</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
@@ -5256,7 +5256,7 @@
         <v>268</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
@@ -5284,7 +5284,7 @@
         <v>268</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
@@ -5298,7 +5298,7 @@
         <v>268</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
@@ -5312,7 +5312,7 @@
         <v>268</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
@@ -5354,7 +5354,7 @@
         <v>268</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
@@ -5396,7 +5396,7 @@
         <v>268</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
@@ -5410,7 +5410,7 @@
         <v>268</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
@@ -5480,7 +5480,7 @@
         <v>334</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
@@ -5522,7 +5522,7 @@
         <v>334</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
@@ -5592,7 +5592,7 @@
         <v>348</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
@@ -5606,7 +5606,7 @@
         <v>348</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
@@ -5620,7 +5620,7 @@
         <v>348</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
@@ -5648,7 +5648,7 @@
         <v>348</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
@@ -5718,7 +5718,7 @@
         <v>348</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
@@ -5732,7 +5732,7 @@
         <v>348</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
@@ -5984,7 +5984,7 @@
         <v>348</v>
       </c>
       <c r="D249" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
@@ -5998,7 +5998,7 @@
         <v>348</v>
       </c>
       <c r="D250" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
@@ -6040,7 +6040,7 @@
         <v>348</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
@@ -6054,7 +6054,7 @@
         <v>348</v>
       </c>
       <c r="D254" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
@@ -6208,7 +6208,7 @@
         <v>348</v>
       </c>
       <c r="D265" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
@@ -6236,7 +6236,7 @@
         <v>348</v>
       </c>
       <c r="D267" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
@@ -6628,7 +6628,7 @@
         <v>348</v>
       </c>
       <c r="D295" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
@@ -6656,7 +6656,7 @@
         <v>348</v>
       </c>
       <c r="D297" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.2">
@@ -6684,7 +6684,7 @@
         <v>348</v>
       </c>
       <c r="D299" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.2">
@@ -6698,7 +6698,7 @@
         <v>348</v>
       </c>
       <c r="D300" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
@@ -6754,7 +6754,7 @@
         <v>348</v>
       </c>
       <c r="D304" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.2">
@@ -6866,7 +6866,7 @@
         <v>348</v>
       </c>
       <c r="D312" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.2">
@@ -6880,7 +6880,7 @@
         <v>348</v>
       </c>
       <c r="D313" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.2">
@@ -6950,7 +6950,7 @@
         <v>348</v>
       </c>
       <c r="D318" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.2">
@@ -7062,7 +7062,7 @@
         <v>348</v>
       </c>
       <c r="D326" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.2">
@@ -7146,7 +7146,7 @@
         <v>348</v>
       </c>
       <c r="D332" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.2">
@@ -7202,7 +7202,7 @@
         <v>420</v>
       </c>
       <c r="D336" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.2">
@@ -7230,7 +7230,7 @@
         <v>420</v>
       </c>
       <c r="D338" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.2">
@@ -7244,7 +7244,7 @@
         <v>420</v>
       </c>
       <c r="D339" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.2">
@@ -7300,7 +7300,7 @@
         <v>420</v>
       </c>
       <c r="D343" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.2">
@@ -7328,7 +7328,7 @@
         <v>420</v>
       </c>
       <c r="D345" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.2">
@@ -7342,7 +7342,7 @@
         <v>420</v>
       </c>
       <c r="D346" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.2">
@@ -7356,7 +7356,7 @@
         <v>420</v>
       </c>
       <c r="D347" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.2">
@@ -7384,7 +7384,7 @@
         <v>420</v>
       </c>
       <c r="D349" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.2">
@@ -7412,7 +7412,7 @@
         <v>420</v>
       </c>
       <c r="D351" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.2">
@@ -7426,7 +7426,7 @@
         <v>420</v>
       </c>
       <c r="D352" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.2">
@@ -7454,7 +7454,7 @@
         <v>420</v>
       </c>
       <c r="D354" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.2">
@@ -7468,7 +7468,7 @@
         <v>420</v>
       </c>
       <c r="D355" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.2">
@@ -7482,7 +7482,7 @@
         <v>420</v>
       </c>
       <c r="D356" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.2">
@@ -7496,7 +7496,7 @@
         <v>420</v>
       </c>
       <c r="D357" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.2">
@@ -7510,7 +7510,7 @@
         <v>420</v>
       </c>
       <c r="D358" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.2">
@@ -7524,7 +7524,7 @@
         <v>420</v>
       </c>
       <c r="D359" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.2">
@@ -7538,7 +7538,7 @@
         <v>420</v>
       </c>
       <c r="D360" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.2">
@@ -7552,7 +7552,7 @@
         <v>420</v>
       </c>
       <c r="D361" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.2">
@@ -7594,7 +7594,7 @@
         <v>420</v>
       </c>
       <c r="D364" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.2">
@@ -7664,7 +7664,7 @@
         <v>420</v>
       </c>
       <c r="D369" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.2">
@@ -7678,7 +7678,7 @@
         <v>420</v>
       </c>
       <c r="D370" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.2">
@@ -7692,7 +7692,7 @@
         <v>420</v>
       </c>
       <c r="D371" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.2">
@@ -7706,7 +7706,7 @@
         <v>420</v>
       </c>
       <c r="D372" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.2">
@@ -7720,7 +7720,7 @@
         <v>420</v>
       </c>
       <c r="D373" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.2">
@@ -7776,7 +7776,7 @@
         <v>504</v>
       </c>
       <c r="D377" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.2">
@@ -7790,7 +7790,7 @@
         <v>504</v>
       </c>
       <c r="D378" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.2">
@@ -7804,7 +7804,7 @@
         <v>504</v>
       </c>
       <c r="D379" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.2">
@@ -7860,7 +7860,7 @@
         <v>504</v>
       </c>
       <c r="D383" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.2">
@@ -7888,7 +7888,7 @@
         <v>504</v>
       </c>
       <c r="D385" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.2">
@@ -7902,7 +7902,7 @@
         <v>504</v>
       </c>
       <c r="D386" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.2">
@@ -8042,7 +8042,7 @@
         <v>504</v>
       </c>
       <c r="D396" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.2">
@@ -8056,7 +8056,7 @@
         <v>504</v>
       </c>
       <c r="D397" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.2">
@@ -8126,7 +8126,7 @@
         <v>504</v>
       </c>
       <c r="D402" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.2">
@@ -8224,7 +8224,7 @@
         <v>504</v>
       </c>
       <c r="D409" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.2">
@@ -8336,7 +8336,7 @@
         <v>555</v>
       </c>
       <c r="D417" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.2">
@@ -8350,7 +8350,7 @@
         <v>555</v>
       </c>
       <c r="D418" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.2">
@@ -8364,7 +8364,7 @@
         <v>556</v>
       </c>
       <c r="D419" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.2">
@@ -8560,7 +8560,7 @@
         <v>559</v>
       </c>
       <c r="D433" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.2">
@@ -8602,7 +8602,7 @@
         <v>559</v>
       </c>
       <c r="D436" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.2">
@@ -8630,7 +8630,7 @@
         <v>559</v>
       </c>
       <c r="D438" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.2">
@@ -8644,7 +8644,7 @@
         <v>559</v>
       </c>
       <c r="D439" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.2">
@@ -8658,7 +8658,7 @@
         <v>559</v>
       </c>
       <c r="D440" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.2">
@@ -8672,7 +8672,7 @@
         <v>559</v>
       </c>
       <c r="D441" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.2">
@@ -8742,7 +8742,7 @@
         <v>559</v>
       </c>
       <c r="D446" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.2">
@@ -8798,7 +8798,7 @@
         <v>597</v>
       </c>
       <c r="D450" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.2">
@@ -8812,7 +8812,7 @@
         <v>597</v>
       </c>
       <c r="D451" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.2">
@@ -8826,7 +8826,7 @@
         <v>597</v>
       </c>
       <c r="D452" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.2">
@@ -8854,7 +8854,7 @@
         <v>611</v>
       </c>
       <c r="D454" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.2">
@@ -8994,7 +8994,7 @@
         <v>611</v>
       </c>
       <c r="D464" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.2">
@@ -9092,7 +9092,7 @@
         <v>614</v>
       </c>
       <c r="D471" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.2">
@@ -9120,7 +9120,7 @@
         <v>614</v>
       </c>
       <c r="D473" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.2">
@@ -9162,7 +9162,7 @@
         <v>627</v>
       </c>
       <c r="D476" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.2">
@@ -9176,7 +9176,7 @@
         <v>627</v>
       </c>
       <c r="D477" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.2">
@@ -9218,7 +9218,7 @@
         <v>627</v>
       </c>
       <c r="D480" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.2">
@@ -9232,7 +9232,7 @@
         <v>627</v>
       </c>
       <c r="D481" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.2">
@@ -9260,7 +9260,7 @@
         <v>632</v>
       </c>
       <c r="D483" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.2">
@@ -9274,7 +9274,7 @@
         <v>632</v>
       </c>
       <c r="D484" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.2">
@@ -9288,7 +9288,7 @@
         <v>632</v>
       </c>
       <c r="D485" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.2">
@@ -9316,7 +9316,7 @@
         <v>640</v>
       </c>
       <c r="D487" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.2">
@@ -9330,7 +9330,7 @@
         <v>640</v>
       </c>
       <c r="D488" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.2">
@@ -9344,7 +9344,7 @@
         <v>640</v>
       </c>
       <c r="D489" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>